<commit_message>
erster Teil geschrieben und verbessert
</commit_message>
<xml_diff>
--- a/Auswertung-MR/Berechnung der Lamordrequenz.xlsx
+++ b/Auswertung-MR/Berechnung der Lamordrequenz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\EFNMR-Remote\Auswertung-MR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D28B0FB-07A6-4E4E-8D62-6E97764DD4BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D18307-4B69-4A59-A053-37F6D59717BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="8325" windowWidth="29040" windowHeight="15840" xr2:uid="{726F7E4B-A8CD-4BD8-8865-895C62E9830F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{726F7E4B-A8CD-4BD8-8865-895C62E9830F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Berde</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -95,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F7B0B9-98DF-4F5B-B7C0-A8C3F081C705}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -489,7 +496,7 @@
         <v>1.1185000000000002E-6</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="G3:I3" si="0">H2*10^(-9)</f>
+        <f t="shared" ref="H3:I3" si="0">H2*10^(-9)</f>
         <v>4.3248800000000005E-5</v>
       </c>
       <c r="I3">
@@ -512,7 +519,7 @@
         <v>908.78903419999995</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="B6:I6" si="1">G3*$C$3</f>
+        <f t="shared" ref="G6:I6" si="1">G3*$C$3</f>
         <v>47.622374500000006</v>
       </c>
       <c r="H6">
@@ -522,6 +529,23 @@
       <c r="I6">
         <f t="shared" si="1"/>
         <v>2054.0464686999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C9" s="1">
+        <v>4.1700000000000001E-10</v>
+      </c>
+      <c r="D9" s="1">
+        <f>1/(H6^2*C9*(2*PI())^2)</f>
+        <v>17.914552724594163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>